<commit_message>
update code after reviewing: - add folder handlers - delete file handleUtil
</commit_message>
<xml_diff>
--- a/documents/NodeJS.xlsx
+++ b/documents/NodeJS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="370">
   <si>
     <t>A. Common</t>
   </si>
@@ -1888,9 +1888,6 @@
     <t>chứa các câu truy vấn SQL</t>
   </si>
   <si>
-    <t>chứa các xử lý common theo từng loại: handleUtil, jwtUtil…</t>
-  </si>
-  <si>
     <t>xử lý check validate data</t>
   </si>
   <si>
@@ -2074,6 +2071,15 @@
   </si>
   <si>
     <t xml:space="preserve">+ secretToken: </t>
+  </si>
+  <si>
+    <t>chứa các xử lý common theo từng loại: jwtUtil…</t>
+  </si>
+  <si>
+    <t>handlers:</t>
+  </si>
+  <si>
+    <t>handle các xử lý như error, success, authentication</t>
   </si>
 </sst>
 </file>
@@ -2703,44 +2709,6 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>342629</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>56524</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="609600" y="571500"/>
-          <a:ext cx="2171429" cy="5009524"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -3597,6 +3565,44 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304533</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>8905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="609600" y="571500"/>
+          <a:ext cx="2133333" cy="4961905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4792,8 +4798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,8 +5269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:O45"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="S39" sqref="S39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5353,7 +5359,7 @@
         <v>301</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>309</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -5361,20 +5367,28 @@
         <v>302</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>312</v>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
@@ -5470,65 +5484,65 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.25">
       <c r="G22" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C25" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.25">
       <c r="M27" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.25">
       <c r="M29" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N30" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N31" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.25">
       <c r="N32" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="49" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C49" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="51" spans="3:17" x14ac:dyDescent="0.25">
       <c r="M51" s="17" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="N51" s="17"/>
       <c r="O51" s="17"/>
@@ -5537,57 +5551,57 @@
     </row>
     <row r="52" spans="3:17" x14ac:dyDescent="0.25">
       <c r="M52" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="59" spans="3:17" x14ac:dyDescent="0.25">
       <c r="M59" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="3:17" x14ac:dyDescent="0.25">
       <c r="N60" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="3:17" x14ac:dyDescent="0.25">
       <c r="N61" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="62" spans="3:17" x14ac:dyDescent="0.25">
       <c r="N62" s="16" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C83" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="84" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D84" s="16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="86" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L86" s="16" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="103" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D103" s="1" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="105" spans="4:12" x14ac:dyDescent="0.25">
       <c r="L105" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="106" spans="4:12" x14ac:dyDescent="0.25">
       <c r="L106" s="16" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="108" spans="4:12" x14ac:dyDescent="0.25">
@@ -5595,97 +5609,97 @@
     </row>
     <row r="120" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D120" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="121" spans="3:12" x14ac:dyDescent="0.25">
       <c r="E121" s="1" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="123" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C123" s="1" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="125" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L125" s="16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C159" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="182" spans="3:12" x14ac:dyDescent="0.25">
       <c r="D182" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="184" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C184" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="186" spans="3:12" x14ac:dyDescent="0.25">
       <c r="L186" s="16" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="222" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C222" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="237" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D237" s="16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="239" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C239" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="241" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L241" s="16" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="242" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L242" s="16" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="243" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M243" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="244" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M244" s="16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="245" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M245" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="246" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M246" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="247" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M247" s="16" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="248" spans="12:13" x14ac:dyDescent="0.25">
       <c r="M248" s="16" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
   </sheetData>
@@ -5698,7 +5712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C22:O122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O51" sqref="O51"/>
     </sheetView>
   </sheetViews>
@@ -5709,57 +5723,57 @@
   <sheetData>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="40" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C40" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="42" spans="3:15" x14ac:dyDescent="0.25">
       <c r="N42" s="16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="44" spans="3:15" x14ac:dyDescent="0.25">
       <c r="O44" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="3:15" x14ac:dyDescent="0.25">
       <c r="O45" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="3:15" x14ac:dyDescent="0.25">
       <c r="O46" s="19" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" spans="3:15" x14ac:dyDescent="0.25">
       <c r="O47" s="19" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O49" s="16" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O50" s="16" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C82" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C122" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>

</xml_diff>